<commit_message>
New way to average
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12900" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8472" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cube 1" sheetId="1" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,7 +433,7 @@
         <v>1300</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -447,7 +447,7 @@
         <v>633.33333333333326</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -461,7 +461,7 @@
         <v>300</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C33"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1415,7 +1415,7 @@
         <v>1300</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -1429,7 +1429,7 @@
         <v>633.33333333333326</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -1443,7 +1443,7 @@
         <v>300</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C33"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,7 +1917,7 @@
         <v>1300</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -1931,7 +1931,7 @@
         <v>633.33333333333326</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -1945,7 +1945,7 @@
         <v>300</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -2389,7 +2389,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>